<commit_message>
move example_sds_dataset to resources
</commit_message>
<xml_diff>
--- a/resources/example_sds_dataset/dataset_description.xlsx
+++ b/resources/example_sds_dataset/dataset_description.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,35 +456,40 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Value 2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Value 3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value n</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Value 1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Value 2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Value 3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Value 4</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Value 5</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Value 6</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Value 7</t>
         </is>
@@ -518,6 +523,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -540,13 +546,18 @@
           <t>experimental</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Experimental</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -564,6 +575,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -583,7 +595,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Dynamic contrast-enhanced magnetic resonance images of breast cancer patients with tumor locations (Duke-Breast-Cancer-MRI)</t>
+          <t>Duke University DCE-MRI of breast cancer patients</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -593,6 +605,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -612,10 +625,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Background Recent studies showed preliminary data on associations of MRI-based imaging phenotypes of breast tumours with breast cancer molecular, genomic, and related characteristics. In this study, we present a comprehensive analysis of this relationship.
-    Methods We analysed a set of 922 patients with invasive breast cancer and pre-operative MRI. The MRIs were analysed by a computer algorithm to extract 529 features of the tumour and the surrounding tissue. Machine-learning-based models based on the imaging features were trained using a portion of the data (461 patients) to predict the following molecular, genomic, and proliferation characteristics: tumour surrogate molecular subtype, oestrogen receptor, progesterone receptor and human epidermal growth factor status, as well as a tumour proliferation marker (Ki-67). Trained models were evaluated on the set of the remaining 461 patients.
-    Results Multivariate models were predictive of Luminal A subtype with AUC = 0.697 (95% CI: 0.647–0.746, p &lt; .0001), triple negative breast cancer with AUC = 0.654 (95% CI: 0.589–0.727, p &lt; .0001), ER status with AUC = 0.649 (95% CI: 0.591–0.705, p &lt; .001), and PR status with AUC = 0.622 (95% CI: 0.569–0.674, p &lt; .0001). Associations between individual features and subtypes we also found.
-    Conclusions There is a moderate association between tumour molecular biomarkers and algorithmically assessed imaging features.</t>
+          <t>Retrospective collection of MRI from 922 biopsy-confirmed invasive breast cancer patients.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -625,6 +635,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -658,6 +669,7 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -683,6 +695,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -708,6 +721,7 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -725,6 +739,7 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -744,7 +759,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Breast MRI is a common image modality to assess the extent of disease in breast cancer patients. Recent studies show that MRI has a potential in prognosis of patients’ short and long-term outcomes as well as predicting pathological and genomic features of the tumors. However, large, well annotated datasets are needed to make further progress in the field. We share such a dataset here.</t>
+          <t>Breast MRI is a medical image modality used to assess the extent of disease in breast cancer patients. Recent studies show that MRI has a potential in prognosis of patients’ short and long-term outcomes as well as predicting pathological and genomic features of the tumors. However, large, well annotated datasets are needed to make further progress in the field. We share such a dataset here.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -754,6 +769,7 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -773,11 +789,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>In terms of design, the dataset is a single-institutional, retrospective collection of 922 biopsy-confirmed invasive breast cancer patients, over a decade, having the following data components:
-    Demographic, clinical, pathology, treatment, outcomes, and genomic data: Collected from a variety of sources including clinical notes, radiology report, and pathology reports and has served as a source for multiple published papers on radiogenomics, outcomes prediction, and other areas.
-    Pre-operative dynamic contrast enhanced (DCE)-MRI: Downloaded from PACS systems and de-identified for The Cancer Imaging Archive (TCIA) release. These include axial breast MRI images acquired by 1.5T or 3T scanners in the prone positions. Following MRI sequences are shared in DICOM format: a non-fat saturated T1-weighted sequence, a fat-saturated gradient echo T1-weighted pre-contrast sequence, and mostly three to four post-contrast sequences.
-    Locations of lesions in DCE-MRI: Annotations on the DCE-MRI images by radiologists.
-    Imaging features from DCE-MRI: A set of 529 computer-extracted imaging features by inhouse software. These features represent a variety of imaging characteristics including size, shape, texture, and enhancement of both the tumor and the surrounding tissue, which is combined of features commonly published in the literature, as well as the features developed in our lab.</t>
+          <t>This dataset is a single-institutional, retrospective collection of 922 biopsy-confirmed invasive breast cancer patients, over a decade, specifically pre-operative dynamic contrast enhanced (DCE)-MRI that were downloaded from PACS systems and de-identified for The Cancer Imaging Archive (TCIA) release. These include axial breast MRI images acquired by 1.5T or 3T scanners in the prone positions. The following MRI sequences are shared in DICOM format: a non-fat saturated T1-weighted sequence, a fat-saturated gradient echo T1-weighted pre-contrast sequence, and mostly three to four post-contrast sequences.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -787,6 +799,7 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -806,7 +819,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>There is a moderate association between tumour molecular biomarkers and algorithmically assessed imaging features.</t>
+          <t>Data collected for subsequent analysis.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -816,6 +829,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -864,6 +878,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -883,7 +898,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Machine-learning</t>
+          <t>Imaging</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -893,6 +908,7 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -912,7 +928,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>We analysed a set of 922 patients with invasive breast cancer and pre-operative MRI. The MRIs were analysed by a computer algorithm to extract 529 features of the tumour and the surrounding tissue. Machine-learning-based models based on the imaging features were trained using a portion of the data (461 patients) to predict the following molecular, genomic, and proliferation characteristics: tumour surrogate molecular subtype, oestrogen receptor, progesterone receptor and human epidermal growth factor status, as well as a tumour proliferation marker (Ki-67). Trained models were evaluated on the set of the remaining 461 patients.</t>
+          <t>MRI</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -922,6 +938,7 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -939,11 +956,7 @@
           <t>My SPARC research study</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Dynamic contrast-enhanced magnetic resonance images of breast cancer patients with tumor locations (Duke-Breast-Cancer-MRI)</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -951,6 +964,7 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -968,6 +982,7 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1021,6 +1036,7 @@
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1074,6 +1090,7 @@
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1127,6 +1144,7 @@
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1166,40 +1184,21 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Researcher</t>
+          <t>PrincipalInvestigator</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
+          <t>CorrespondingAuthor</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1217,6 +1216,7 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1236,16 +1236,25 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+          <t>Protocol for dataset</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Paper for dataset</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Not Defined</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1304,16 +1313,25 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>HasProtocol</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>IsDescribedBy</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Not Defined</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1333,7 +1351,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ID2350</t>
+          <t>Not Defined</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1343,6 +1361,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1362,7 +1381,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12L digital twin UUID</t>
+          <t>Not Defined</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1372,6 +1391,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1389,6 +1409,7 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1405,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -1414,6 +1435,7 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1430,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -1439,6 +1461,7 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updating raw and sds dataset for tutorials
</commit_message>
<xml_diff>
--- a/resources/example_sds_dataset/dataset_description.xlsx
+++ b/resources/example_sds_dataset/dataset_description.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,35 +456,40 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Value 2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Value 3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Value n</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Value 1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Value 2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Value 3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Value 4</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Value 5</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Value 6</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Value 7</t>
         </is>
@@ -518,6 +523,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -540,13 +546,18 @@
           <t>experimental</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Experimental</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -564,6 +575,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -583,7 +595,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Dynamic contrast-enhanced magnetic resonance images of breast cancer patients with tumor locations (Duke-Breast-Cancer-MRI)</t>
+          <t>Duke University DCE-MRI of breast cancer patients</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -593,6 +605,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -612,10 +625,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Background Recent studies showed preliminary data on associations of MRI-based imaging phenotypes of breast tumours with breast cancer molecular, genomic, and related characteristics. In this study, we present a comprehensive analysis of this relationship.
-    Methods We analysed a set of 922 patients with invasive breast cancer and pre-operative MRI. The MRIs were analysed by a computer algorithm to extract 529 features of the tumour and the surrounding tissue. Machine-learning-based models based on the imaging features were trained using a portion of the data (461 patients) to predict the following molecular, genomic, and proliferation characteristics: tumour surrogate molecular subtype, oestrogen receptor, progesterone receptor and human epidermal growth factor status, as well as a tumour proliferation marker (Ki-67). Trained models were evaluated on the set of the remaining 461 patients.
-    Results Multivariate models were predictive of Luminal A subtype with AUC = 0.697 (95% CI: 0.647–0.746, p &lt; .0001), triple negative breast cancer with AUC = 0.654 (95% CI: 0.589–0.727, p &lt; .0001), ER status with AUC = 0.649 (95% CI: 0.591–0.705, p &lt; .001), and PR status with AUC = 0.622 (95% CI: 0.569–0.674, p &lt; .0001). Associations between individual features and subtypes we also found.
-    Conclusions There is a moderate association between tumour molecular biomarkers and algorithmically assessed imaging features.</t>
+          <t>Retrospective collection of MRI from 922 biopsy-confirmed invasive breast cancer patients.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -625,6 +635,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -658,6 +669,7 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -683,6 +695,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -708,6 +721,7 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -725,6 +739,7 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -744,7 +759,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Breast MRI is a common image modality to assess the extent of disease in breast cancer patients. Recent studies show that MRI has a potential in prognosis of patients’ short and long-term outcomes as well as predicting pathological and genomic features of the tumors. However, large, well annotated datasets are needed to make further progress in the field. We share such a dataset here.</t>
+          <t>Breast MRI is a medical image modality used to assess the extent of disease in breast cancer patients. Recent studies show that MRI has a potential in prognosis of patients’ short and long-term outcomes as well as predicting pathological and genomic features of the tumors. However, large, well annotated datasets are needed to make further progress in the field. We share such a dataset here.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -754,6 +769,7 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -773,11 +789,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>In terms of design, the dataset is a single-institutional, retrospective collection of 922 biopsy-confirmed invasive breast cancer patients, over a decade, having the following data components:
-    Demographic, clinical, pathology, treatment, outcomes, and genomic data: Collected from a variety of sources including clinical notes, radiology report, and pathology reports and has served as a source for multiple published papers on radiogenomics, outcomes prediction, and other areas.
-    Pre-operative dynamic contrast enhanced (DCE)-MRI: Downloaded from PACS systems and de-identified for The Cancer Imaging Archive (TCIA) release. These include axial breast MRI images acquired by 1.5T or 3T scanners in the prone positions. Following MRI sequences are shared in DICOM format: a non-fat saturated T1-weighted sequence, a fat-saturated gradient echo T1-weighted pre-contrast sequence, and mostly three to four post-contrast sequences.
-    Locations of lesions in DCE-MRI: Annotations on the DCE-MRI images by radiologists.
-    Imaging features from DCE-MRI: A set of 529 computer-extracted imaging features by inhouse software. These features represent a variety of imaging characteristics including size, shape, texture, and enhancement of both the tumor and the surrounding tissue, which is combined of features commonly published in the literature, as well as the features developed in our lab.</t>
+          <t>This dataset is a single-institutional, retrospective collection of 922 biopsy-confirmed invasive breast cancer patients, over a decade, specifically pre-operative dynamic contrast enhanced (DCE)-MRI that were downloaded from PACS systems and de-identified for The Cancer Imaging Archive (TCIA) release. These include axial breast MRI images acquired by 1.5T or 3T scanners in the prone positions. The following MRI sequences are shared in DICOM format: a non-fat saturated T1-weighted sequence, a fat-saturated gradient echo T1-weighted pre-contrast sequence, and mostly three to four post-contrast sequences.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -787,6 +799,7 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -806,7 +819,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>There is a moderate association between tumour molecular biomarkers and algorithmically assessed imaging features.</t>
+          <t>Data collected for subsequent analysis.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -816,6 +829,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -864,6 +878,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -883,7 +898,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Machine-learning</t>
+          <t>Imaging</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -893,6 +908,7 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -912,7 +928,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>We analysed a set of 922 patients with invasive breast cancer and pre-operative MRI. The MRIs were analysed by a computer algorithm to extract 529 features of the tumour and the surrounding tissue. Machine-learning-based models based on the imaging features were trained using a portion of the data (461 patients) to predict the following molecular, genomic, and proliferation characteristics: tumour surrogate molecular subtype, oestrogen receptor, progesterone receptor and human epidermal growth factor status, as well as a tumour proliferation marker (Ki-67). Trained models were evaluated on the set of the remaining 461 patients.</t>
+          <t>MRI</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -922,6 +938,7 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -939,11 +956,7 @@
           <t>My SPARC research study</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Dynamic contrast-enhanced magnetic resonance images of breast cancer patients with tumor locations (Duke-Breast-Cancer-MRI)</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -951,6 +964,7 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -968,6 +982,7 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1021,6 +1036,7 @@
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1074,6 +1090,7 @@
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1127,6 +1144,7 @@
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1166,40 +1184,21 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Researcher</t>
+          <t>PrincipalInvestigator</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Researcher</t>
-        </is>
-      </c>
+          <t>CorrespondingAuthor</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1217,6 +1216,7 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1236,16 +1236,25 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+          <t>Protocol for dataset</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Paper for dataset</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Not Defined</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1304,16 +1313,25 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>HasProtocol</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>IsDescribedBy</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Not Defined</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1333,7 +1351,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>ID2350</t>
+          <t>Not Defined</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1343,6 +1361,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1362,7 +1381,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12L digital twin UUID</t>
+          <t>Not Defined</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1372,6 +1391,7 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1389,6 +1409,7 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1405,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -1414,6 +1435,7 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1430,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -1439,6 +1461,7 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>